<commit_message>
Add ratio and quarter pts into xlsx file
</commit_message>
<xml_diff>
--- a/basketBallRecorder/spreadsheet_for_boxScore.xlsx
+++ b/basketBallRecorder/spreadsheet_for_boxScore.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>TO</t>
   </si>
@@ -85,10 +85,6 @@
   </si>
   <si>
     <t>4th</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>total score</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -516,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -590,9 +586,7 @@
       <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="X1" s="2"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="1"/>

</xml_diff>

<commit_message>
Upload boxscore xlsx file from menu page
</commit_message>
<xml_diff>
--- a/basketBallRecorder/spreadsheet_for_boxScore.xlsx
+++ b/basketBallRecorder/spreadsheet_for_boxScore.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>TO</t>
   </si>
@@ -70,22 +70,6 @@
   </si>
   <si>
     <t>PTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2nd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3rd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4th</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -159,13 +143,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -510,18 +497,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X31"/>
+  <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="A1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="1" max="28" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:31">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -573,22 +560,22 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="2"/>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+    </row>
+    <row r="2" spans="1:31">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -611,8 +598,17 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -635,8 +631,17 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -659,8 +664,17 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -683,8 +697,17 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -707,9 +730,17 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
-      <c r="W6" s="2"/>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="W6" s="3"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -732,8 +763,17 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -756,8 +796,17 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -780,8 +829,17 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -804,8 +862,17 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -828,8 +895,17 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+    </row>
+    <row r="12" spans="1:31">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -852,8 +928,17 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+    </row>
+    <row r="13" spans="1:31">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -876,8 +961,17 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+    </row>
+    <row r="14" spans="1:31">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -900,8 +994,17 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+    </row>
+    <row r="15" spans="1:31">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -924,8 +1027,17 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+    </row>
+    <row r="16" spans="1:31">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -948,8 +1060,17 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -972,8 +1093,17 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+    </row>
+    <row r="18" spans="1:31">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -996,8 +1126,17 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+    </row>
+    <row r="19" spans="1:31">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1020,8 +1159,17 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+    </row>
+    <row r="20" spans="1:31">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1044,8 +1192,17 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+    </row>
+    <row r="21" spans="1:31">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1068,8 +1225,17 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+    </row>
+    <row r="22" spans="1:31">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1092,8 +1258,17 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+    </row>
+    <row r="23" spans="1:31">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1116,8 +1291,17 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+    </row>
+    <row r="24" spans="1:31">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1140,8 +1324,17 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+    </row>
+    <row r="25" spans="1:31">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1164,8 +1357,17 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
-    </row>
-    <row r="26" spans="1:22">
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+    </row>
+    <row r="26" spans="1:31">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1188,8 +1390,17 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
-    </row>
-    <row r="27" spans="1:22">
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+    </row>
+    <row r="27" spans="1:31">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1212,8 +1423,17 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
-    </row>
-    <row r="28" spans="1:22">
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+    </row>
+    <row r="28" spans="1:31">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1236,8 +1456,17 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
-    </row>
-    <row r="29" spans="1:22">
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+    </row>
+    <row r="29" spans="1:31">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1260,8 +1489,17 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
-    </row>
-    <row r="30" spans="1:22">
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+    </row>
+    <row r="30" spans="1:31">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1284,8 +1522,17 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
-    </row>
-    <row r="31" spans="1:22">
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+    </row>
+    <row r="31" spans="1:31">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1308,6 +1555,79 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+    </row>
+    <row r="32" spans="1:31">
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+    </row>
+    <row r="33" spans="18:31">
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+    </row>
+    <row r="34" spans="18:31">
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+    </row>
+    <row r="35" spans="18:31">
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>